<commit_message>
added game 2 and 3 stats. added OPS
</commit_message>
<xml_diff>
--- a/softballStats.xlsx
+++ b/softballStats.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apanday\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anujp_000\Dropbox\R Directory\Softball Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="3225" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="3225"/>
   </bookViews>
   <sheets>
     <sheet name="softballStats" sheetId="1" r:id="rId1"/>
     <sheet name="Game 1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>Anuj</t>
   </si>
@@ -97,12 +97,15 @@
   </si>
   <si>
     <t>Rank</t>
+  </si>
+  <si>
+    <t>OPS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +467,7 @@
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -498,512 +501,567 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f>SUM(D2:G2)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I2">
-        <f>1*D2+2*E2+3*F2+4*G2</f>
-        <v>2</v>
+        <f>D2*1+E2*2+F2*3+G2*4</f>
+        <v>15</v>
       </c>
       <c r="J2" s="1">
         <f>H2/C2</f>
-        <v>0.66666666666666663</v>
+        <v>0.9</v>
       </c>
       <c r="K2" s="1">
         <f>I2/C2</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+      <c r="L2" s="1">
+        <f>SUM(J2:K2)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H14" si="0">SUM(D3:G3)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I14" si="1">1*D3+2*E3+3*F3+4*G3</f>
-        <v>3</v>
+        <f t="shared" ref="I3:I14" si="1">D3*1+E3*2+F3*3+G3*4</f>
+        <v>8</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J14" si="2">H3/C3</f>
-        <v>0.75</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="K3" s="1">
         <f t="shared" ref="K3:K14" si="3">I3/C3</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L14" si="4">SUM(J3:K3)</f>
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="3"/>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.2222222222222223</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2222222222222223</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="4"/>
+        <v>1.8571428571428572</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="4"/>
+        <v>1.8333333333333335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
         <v>4</v>
       </c>
-      <c r="J5" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="4"/>
+        <v>1.8333333333333335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="4"/>
+        <v>1.8333333333333335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="4"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J11" s="1">
         <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
-      <c r="K6" s="1">
-        <f t="shared" si="3"/>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="K11" s="1">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="2"/>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="4"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="3"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="4"/>
+        <v>1.1111111111111112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.375</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="3"/>
+        <v>0.375</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="4"/>
         <v>0.75</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="3"/>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="2"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="3"/>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K11" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K12" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K13" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K14" s="1" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -1015,9 +1073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>